<commit_message>
Add bathymetry and beach profile data
</commit_message>
<xml_diff>
--- a/model_summary.xlsx
+++ b/model_summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z3541792_ad_unsw_edu_au/Documents/Documents/GitHub/ShoreModel_Benchmark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="493" documentId="11_F25DC773A252ABDACC1048DD819946C45ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC2DAEA2-457D-485D-B03E-83152A1634CE}"/>
+  <xr:revisionPtr revIDLastSave="506" documentId="11_F25DC773A252ABDACC1048DD819946C45ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89C48F4B-B159-43CF-9FA8-06F8BC23CEC0}"/>
   <bookViews>
-    <workbookView xWindow="3017" yWindow="3017" windowWidth="16457" windowHeight="9506" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="107">
   <si>
     <t>Model Name</t>
   </si>
@@ -331,6 +331,21 @@
   </si>
   <si>
     <t>SARIMAX_AG</t>
+  </si>
+  <si>
+    <t>Submission Type</t>
+  </si>
+  <si>
+    <t>Submission</t>
+  </si>
+  <si>
+    <t>Resubmission</t>
+  </si>
+  <si>
+    <t>ShoreForLogSpiral_BD</t>
+  </si>
+  <si>
+    <t>Bixuan Dong</t>
   </si>
 </sst>
 </file>
@@ -684,24 +699,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C26" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.3046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="25.15234375" customWidth="1"/>
-    <col min="9" max="9" width="11.53515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.84375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.53515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="36.3046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="25.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -717,8 +733,9 @@
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -755,11 +772,14 @@
       <c r="L2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -781,8 +801,11 @@
       <c r="I3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -816,8 +839,11 @@
       <c r="K4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -851,8 +877,11 @@
       <c r="K5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>90</v>
       </c>
@@ -883,8 +912,11 @@
       <c r="K6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>91</v>
       </c>
@@ -915,8 +947,11 @@
       <c r="K7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>92</v>
       </c>
@@ -947,8 +982,11 @@
       <c r="K8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>93</v>
       </c>
@@ -979,8 +1017,11 @@
       <c r="K9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1014,8 +1055,11 @@
       <c r="K10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>94</v>
       </c>
@@ -1049,8 +1093,11 @@
       <c r="K11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1079,8 +1126,11 @@
       <c r="J12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1117,8 +1167,11 @@
       <c r="L13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1155,8 +1208,11 @@
       <c r="L14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1193,8 +1249,11 @@
       <c r="L15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -1219,8 +1278,11 @@
       <c r="J16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -1248,8 +1310,11 @@
       <c r="K17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1280,8 +1345,11 @@
       <c r="J18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1309,8 +1377,11 @@
       <c r="J19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>81</v>
       </c>
@@ -1339,10 +1410,13 @@
         <v>16</v>
       </c>
       <c r="M20" t="s">
+        <v>103</v>
+      </c>
+      <c r="N20" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>78</v>
       </c>
@@ -1367,8 +1441,11 @@
       <c r="J21" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>77</v>
       </c>
@@ -1402,8 +1479,11 @@
       <c r="K22" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>99</v>
       </c>
@@ -1437,8 +1517,11 @@
       <c r="K23" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M23" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1469,8 +1552,11 @@
       <c r="K24" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>101</v>
       </c>
@@ -1493,8 +1579,11 @@
         <v>16</v>
       </c>
       <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -1519,8 +1608,11 @@
       <c r="I26" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M26" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1551,8 +1643,11 @@
       <c r="K27" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1577,8 +1672,11 @@
       <c r="I28" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M28" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -1615,8 +1713,11 @@
       <c r="L29" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M29" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1648,8 +1749,11 @@
       <c r="K30" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>100</v>
       </c>
@@ -1681,8 +1785,11 @@
       <c r="K31" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M31" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>74</v>
       </c>
@@ -1713,8 +1820,11 @@
       <c r="K32" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="M32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>24</v>
       </c>
@@ -1742,8 +1852,11 @@
       <c r="I33" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="M33" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1777,8 +1890,11 @@
       <c r="K34" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="M34" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>96</v>
       </c>
@@ -1803,8 +1919,11 @@
       <c r="J35" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="M35" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>97</v>
       </c>
@@ -1829,8 +1948,11 @@
       <c r="J36" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="M36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>73</v>
       </c>
@@ -1861,8 +1983,11 @@
       <c r="K37" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="M37" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -1887,8 +2012,11 @@
       <c r="I38" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="M38" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>71</v>
       </c>
@@ -1916,8 +2044,11 @@
       <c r="J39" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="M39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -1942,8 +2073,11 @@
       <c r="I40" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="M40" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>68</v>
       </c>
@@ -1973,6 +2107,35 @@
       </c>
       <c r="J41" t="s">
         <v>16</v>
+      </c>
+      <c r="M41" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>105</v>
+      </c>
+      <c r="B42" t="s">
+        <v>106</v>
+      </c>
+      <c r="C42" t="s">
+        <v>57</v>
+      </c>
+      <c r="D42" t="s">
+        <v>58</v>
+      </c>
+      <c r="E42" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" t="s">
+        <v>13</v>
+      </c>
+      <c r="I42" t="s">
+        <v>16</v>
+      </c>
+      <c r="M42" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>